<commit_message>
add modes and update vocab file
</commit_message>
<xml_diff>
--- a/project/vocab.xlsx
+++ b/project/vocab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilb\Projects\Oboeru\Oboeru\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC87EC3-CA6B-4000-B9DC-B26F90A6CC8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425C6B15-7337-4967-B175-B114B9440167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75A4A7FE-AA9B-48C2-A5CA-A82ACC0BB528}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6933" uniqueCount="3028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6933" uniqueCount="3027">
   <si>
     <t>わたし</t>
   </si>
@@ -9156,9 +9156,6 @@
   </si>
   <si>
     <t>さいきん</t>
-  </si>
-  <si>
-    <t>kai</t>
   </si>
   <si>
     <t>pos</t>
@@ -9709,8 +9706,8 @@
   <dimension ref="A1:I1206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F553" sqref="F553"/>
+      <pane ySplit="1" topLeftCell="A395" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F406" sqref="F406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9728,31 +9725,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>3019</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3018</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>3022</v>
+      </c>
+      <c r="D1" t="s">
         <v>3020</v>
       </c>
-      <c r="B1" t="s">
-        <v>3019</v>
-      </c>
-      <c r="C1" s="18" t="s">
+      <c r="E1" s="4" t="s">
+        <v>3021</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>3023</v>
       </c>
-      <c r="D1" t="s">
-        <v>3021</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3022</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="12" t="s">
         <v>3024</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" t="s">
         <v>3025</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>3026</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3027</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -16601,7 +16598,7 @@
         <v>827</v>
       </c>
       <c r="F406" s="7" t="s">
-        <v>3018</v>
+        <v>1113</v>
       </c>
       <c r="G406" s="12" t="s">
         <v>1071</v>

</xml_diff>

<commit_message>
Fix lesson number vocab
</commit_message>
<xml_diff>
--- a/project/vocab.xlsx
+++ b/project/vocab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilb\Projects\Oboeru\Oboeru\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425C6B15-7337-4967-B175-B114B9440167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED1172B-3344-4B59-ABF6-B81106C21E06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75A4A7FE-AA9B-48C2-A5CA-A82ACC0BB528}"/>
   </bookViews>
@@ -9706,8 +9706,8 @@
   <dimension ref="A1:I1206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A395" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F406" sqref="F406"/>
+      <pane ySplit="1" topLeftCell="A862" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C879" sqref="C879"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24269,7 +24269,7 @@
     </row>
     <row r="854" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A854" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B854" t="s">
         <v>2648</v>
@@ -24289,7 +24289,7 @@
     </row>
     <row r="855" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A855" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B855" t="s">
         <v>2648</v>
@@ -24306,7 +24306,7 @@
     </row>
     <row r="856" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A856" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B856" t="s">
         <v>2648</v>
@@ -24323,7 +24323,7 @@
     </row>
     <row r="857" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A857" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B857" t="s">
         <v>2648</v>
@@ -24340,7 +24340,7 @@
     </row>
     <row r="858" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A858" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B858" t="s">
         <v>2648</v>
@@ -24357,7 +24357,7 @@
     </row>
     <row r="859" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A859" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B859" t="s">
         <v>2648</v>
@@ -24377,7 +24377,7 @@
     </row>
     <row r="860" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A860" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B860" t="s">
         <v>2645</v>
@@ -24392,7 +24392,7 @@
     </row>
     <row r="861" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A861" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B861" t="s">
         <v>2645</v>
@@ -24410,7 +24410,7 @@
     </row>
     <row r="862" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A862" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B862" t="s">
         <v>2645</v>
@@ -24428,7 +24428,7 @@
     </row>
     <row r="863" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A863" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B863" t="s">
         <v>2645</v>
@@ -24446,7 +24446,7 @@
     </row>
     <row r="864" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A864" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B864" t="s">
         <v>2645</v>
@@ -24464,7 +24464,7 @@
     </row>
     <row r="865" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A865" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B865" t="s">
         <v>2645</v>
@@ -24479,7 +24479,7 @@
     </row>
     <row r="866" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A866" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B866" t="s">
         <v>2645</v>
@@ -24497,7 +24497,7 @@
     </row>
     <row r="867" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A867" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B867" t="s">
         <v>2645</v>
@@ -24512,7 +24512,7 @@
     </row>
     <row r="868" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A868" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B868" t="s">
         <v>2645</v>
@@ -24530,7 +24530,7 @@
     </row>
     <row r="869" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A869" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B869" t="s">
         <v>2645</v>
@@ -24548,7 +24548,7 @@
     </row>
     <row r="870" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A870" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B870" t="s">
         <v>2645</v>
@@ -24563,7 +24563,7 @@
     </row>
     <row r="871" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A871" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B871" t="s">
         <v>1133</v>
@@ -24578,7 +24578,7 @@
     </row>
     <row r="872" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A872" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B872" t="s">
         <v>2646</v>
@@ -24593,7 +24593,7 @@
     </row>
     <row r="873" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A873" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B873" t="s">
         <v>2646</v>
@@ -24608,7 +24608,7 @@
     </row>
     <row r="874" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A874" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B874" t="s">
         <v>2646</v>
@@ -24623,7 +24623,7 @@
     </row>
     <row r="875" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A875" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B875" t="s">
         <v>2646</v>
@@ -24638,7 +24638,7 @@
     </row>
     <row r="876" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A876" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B876" t="s">
         <v>2646</v>
@@ -24653,7 +24653,7 @@
     </row>
     <row r="877" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A877" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B877" t="s">
         <v>2645</v>
@@ -24668,7 +24668,7 @@
     </row>
     <row r="878" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A878" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B878" t="s">
         <v>2645</v>
@@ -24686,7 +24686,7 @@
     </row>
     <row r="879" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A879" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B879" t="s">
         <v>2645</v>
@@ -24701,7 +24701,7 @@
     </row>
     <row r="880" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A880" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B880" t="s">
         <v>2645</v>
@@ -24716,7 +24716,7 @@
     </row>
     <row r="881" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A881" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B881" t="s">
         <v>2645</v>
@@ -36470,8 +36470,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:E356"/>
   <sheetViews>
-    <sheetView topLeftCell="A300" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E356"/>
+    <sheetView topLeftCell="A279" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C338" sqref="C338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>